<commit_message>
complete restructure and rewrite of documentation ready for v2
</commit_message>
<xml_diff>
--- a/inst/extdata/append_tests/invalid_append_01.xlsx
+++ b/inst/extdata/append_tests/invalid_append_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rverity/Dropbox/Bob/Work/My Programs/Mapping/STAVE/inst/extdata/append_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F7F872-E9A9-1948-BBBB-73CDD51589A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8B2FD3-8F99-724C-815F-49B35F804CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1080" windowWidth="31520" windowHeight="18700" activeTab="3" xr2:uid="{A4E9C168-401F-F34B-85A4-C504E7A73195}"/>
+    <workbookView xWindow="780" yWindow="1080" windowWidth="31520" windowHeight="18700" activeTab="1" xr2:uid="{A4E9C168-401F-F34B-85A4-C504E7A73195}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Notes</t>
   </si>
@@ -47,42 +47,18 @@
     <t>This is an example of input data that should fail tests</t>
   </si>
   <si>
-    <t>study_name</t>
-  </si>
-  <si>
-    <t>study_type</t>
-  </si>
-  <si>
-    <t>authors</t>
-  </si>
-  <si>
-    <t>publication_year</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>foo</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1093%2Fgenetics%2F16.2.97</t>
   </si>
   <si>
-    <t>study_key</t>
-  </si>
-  <si>
     <t>country_name</t>
   </si>
   <si>
     <t>site_name</t>
   </si>
   <si>
-    <t>spatial_notes</t>
-  </si>
-  <si>
     <t>collection_start</t>
   </si>
   <si>
@@ -101,9 +77,6 @@
     <t>example data</t>
   </si>
   <si>
-    <t>survey_key</t>
-  </si>
-  <si>
     <t>variant_string</t>
   </si>
   <si>
@@ -132,6 +105,36 @@
   </si>
   <si>
     <t>Specific issue: study_IDs are already present in the corresponding preloaded data</t>
+  </si>
+  <si>
+    <t>study_label</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>access_level</t>
+  </si>
+  <si>
+    <t>contributors</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>reference_year</t>
+  </si>
+  <si>
+    <t>location_method</t>
+  </si>
+  <si>
+    <t>location_notes</t>
+  </si>
+  <si>
+    <t>time_method</t>
+  </si>
+  <si>
+    <t>public</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -545,10 +548,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{913D86B1-4503-0D4D-8A9D-3BCCCF42F647}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,35 +559,38 @@
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCF84CB1-9532-2C43-A7F8-683871878F9F}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -608,47 +614,53 @@
     <col min="8" max="10" width="14.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -656,14 +668,15 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -675,38 +688,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E51D5F-A46A-0B42-A5D0-47D275C37629}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>